<commit_message>
Update figures and added comparison of screens
</commit_message>
<xml_diff>
--- a/2_Tridimensional screening/analysis/screening_text/gross screens/SUMMARY values.xlsx
+++ b/2_Tridimensional screening/analysis/screening_text/gross screens/SUMMARY values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kvase0-my.sharepoint.com/personal/loudel30_kva_se/Documents/Dokument/GitHub/WEF-GRR-analysis/2_Tridimensional screening/analysis/screening_text/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kvase0-my.sharepoint.com/personal/loudel30_kva_se/Documents/Dokument/GitHub/WEF-GRR-analysis/2_Tridimensional screening/analysis/screening_text/gross screens/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{06E48593-8CA4-DB4E-9FF5-935F180AD992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A916EA0A-7F5B-4442-9AFD-E004A239B93E}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{97D5B879-A007-B64B-8EC2-E32FDA0662EE}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{97D5B879-A007-B64B-8EC2-E32FDA0662EE}"/>
   </bookViews>
   <sheets>
     <sheet name="SDG" sheetId="1" r:id="rId1"/>
@@ -12643,7 +12643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BA6C2D-0F96-C044-828C-1BB3A53DC349}">
   <dimension ref="A9:U189"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A136" activeCellId="1" sqref="A134:R134 A136:R137"/>
     </sheetView>
   </sheetViews>
@@ -14786,8 +14786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9A8D0F-47A4-724E-AB60-0F40DEE641E9}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="A22" sqref="A4:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="15.9"/>

</xml_diff>